<commit_message>
Added Investment Amount in import of remittances
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_remittances.xlsx
+++ b/public/sample_uploads/capital_remittances.xlsx
@@ -231,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -255,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -279,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t xml:space="preserve">Stakeholder *</t>
   </si>
@@ -335,6 +335,9 @@
   </si>
   <si>
     <t xml:space="preserve">Other Fees (Fund Currency)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investment Amont (Fund Currency)</t>
   </si>
   <si>
     <t xml:space="preserve">Remittance Date</t>
@@ -489,15 +492,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -691,10 +694,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -706,10 +709,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.62"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="7" style="1" width="9.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.38"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="13" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="14.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="8.38"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="14" style="1" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,16 +752,19 @@
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>12000</v>
@@ -769,22 +775,25 @@
       <c r="F2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="n">
+      <c r="J2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>30000</v>
@@ -795,22 +804,25 @@
       <c r="F3" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="1" t="n">
+      <c r="J3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="1" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>15000</v>
@@ -821,22 +833,25 @@
       <c r="F4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="1" t="n">
+      <c r="J4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="1" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>12000</v>
@@ -847,22 +862,25 @@
       <c r="F5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="1" t="n">
+      <c r="J5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="1" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>13000</v>
@@ -873,22 +891,25 @@
       <c r="F6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L6" s="1" t="n">
+      <c r="J6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="1" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>13000</v>
@@ -899,22 +920,25 @@
       <c r="F7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L7" s="1" t="n">
+      <c r="J7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="1" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>13000</v>
@@ -925,22 +949,25 @@
       <c r="F8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="1" t="n">
+      <c r="J8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="1" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>13000</v>
@@ -951,16 +978,19 @@
       <c r="F9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L9" s="1" t="n">
+      <c r="J9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="1" t="n">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="K2:K183" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="L2:L183" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Remittance upload tests work
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_remittances.xlsx
+++ b/public/sample_uploads/capital_remittances.xlsx
@@ -337,7 +337,7 @@
     <t xml:space="preserve">Other Fees (Fund Currency)</t>
   </si>
   <si>
-    <t xml:space="preserve">Investment Amont (Fund Currency)</t>
+    <t xml:space="preserve">Investment Amount (Fund Currency)</t>
   </si>
   <si>
     <t xml:space="preserve">Remittance Date</t>
@@ -697,7 +697,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>